<commit_message>
Authorization Checks - done
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -790,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -1030,7 +1030,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="5">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
allAdsController.js message bug fixed That's all from ME :)
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>